<commit_message>
dding files from the 28th of november
</commit_message>
<xml_diff>
--- a/courses/M2.218.13875-89 MAG. Introduction to business management 2223-S1/BP PRESENTATIONS 88+89.xlsx
+++ b/courses/M2.218.13875-89 MAG. Introduction to business management 2223-S1/BP PRESENTATIONS 88+89.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grasi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D24CB4-4C58-443A-96D1-27930D5FBC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3697870B-D18B-4FBC-ADCC-5896F529AADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>15.00 - 15.10</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t xml:space="preserve">UPLOAD YOUR BUSINESS PLAN UNTIL 4TH OF DECEMBER IN THE RESPECTIVE LINK IN THE AULA GLOBAL </t>
+  </si>
+  <si>
+    <t>Pablo Agudo Moreno (100429972) and me, Juan Álvarez Sánchez (100495738)</t>
   </si>
 </sst>
 </file>
@@ -696,7 +699,7 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,7 +735,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>

</xml_diff>